<commit_message>
warehouse with entry processes coniguration completed
</commit_message>
<xml_diff>
--- a/soberano/test_cases/warehouse_with_entry_processes_record_test_cases.xlsx
+++ b/soberano/test_cases/warehouse_with_entry_processes_record_test_cases.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="108" uniqueCount="58">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="107" uniqueCount="57">
   <si>
     <t xml:space="preserve">TC Number</t>
   </si>
@@ -191,9 +191,6 @@
   </si>
   <si>
     <t xml:space="preserve">check w30 data is correctly shown in details panel</t>
-  </si>
-  <si>
-    <t xml:space="preserve">check w31 data is correctly shown in details panel</t>
   </si>
 </sst>
 </file>
@@ -336,10 +333,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:AMJ27"/>
+  <dimension ref="A1:AMJ26"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A9" activeCellId="0" sqref="9:9"/>
+      <selection pane="topLeft" activeCell="A14" activeCellId="0" sqref="14:14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -817,14 +814,6 @@
         <v>56</v>
       </c>
     </row>
-    <row r="27" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A27" s="1" t="n">
-        <v>26</v>
-      </c>
-      <c r="B27" s="1" t="s">
-        <v>57</v>
-      </c>
-    </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.025" bottom="1.025" header="0.7875" footer="0.7875"/>

</xml_diff>